<commit_message>
Fix xlsx loader to load in files
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -356,7 +356,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -364,7 +364,7 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
     <col customWidth="1" min="1" max="2" width="27.75"/>
     <col customWidth="1" min="3" max="3" width="22.63"/>
@@ -387,7 +387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" outlineLevel="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -404,7 +404,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" outlineLevel="1">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
@@ -418,7 +418,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" outlineLevel="1">
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -432,7 +432,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5">
+    <row r="5" outlineLevel="1">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -446,7 +446,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6">
+    <row r="6" outlineLevel="1">
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -460,7 +460,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7">
+    <row r="7" outlineLevel="1">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -474,7 +474,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8">
+    <row r="8" outlineLevel="1">
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
@@ -488,7 +488,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9">
+    <row r="9" outlineLevel="1">
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -502,7 +502,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10">
+    <row r="10" outlineLevel="1">
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>